<commit_message>
New price data for December 2022.
</commit_message>
<xml_diff>
--- a/price_data/data (113).xlsx
+++ b/price_data/data (113).xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
   <si>
     <t>Tidsperiod</t>
   </si>
@@ -378,6 +378,150 @@
   </si>
   <si>
     <t>2022-12-05 23:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 00:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 01:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 02:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 03:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 04:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 05:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 06:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 07:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 08:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 09:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 10:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 11:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 12:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 13:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 14:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 15:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 16:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 17:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 18:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 19:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 20:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 21:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 22:00</t>
+  </si>
+  <si>
+    <t>2022-12-06 23:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 00:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 01:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 02:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 03:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 04:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 05:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 06:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 07:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 08:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 09:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 10:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 11:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 12:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 13:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 14:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 15:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 16:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 17:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 18:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 19:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 20:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 21:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 22:00</t>
+  </si>
+  <si>
+    <t>2022-12-07 23:00</t>
   </si>
 </sst>
 </file>
@@ -422,7 +566,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B122" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B170" headerRowCount="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Tidsperiod"/>
     <tableColumn id="2" name="01 dec 2022 - 07 dec 2022"/>
@@ -433,7 +577,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:B169"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1032,7 +1176,7 @@
         <v>74</v>
       </c>
       <c r="B74" s="0">
-        <v>251.55</v>
+        <v>251.14</v>
       </c>
     </row>
     <row r="75">
@@ -1040,7 +1184,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="0">
-        <v>239.8</v>
+        <v>239.41</v>
       </c>
     </row>
     <row r="76">
@@ -1048,7 +1192,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="0">
-        <v>252.08</v>
+        <v>251.67</v>
       </c>
     </row>
     <row r="77">
@@ -1056,7 +1200,7 @@
         <v>77</v>
       </c>
       <c r="B77" s="0">
-        <v>229.73</v>
+        <v>229.36</v>
       </c>
     </row>
     <row r="78">
@@ -1064,7 +1208,7 @@
         <v>78</v>
       </c>
       <c r="B78" s="0">
-        <v>228.34</v>
+        <v>227.96</v>
       </c>
     </row>
     <row r="79">
@@ -1072,7 +1216,7 @@
         <v>79</v>
       </c>
       <c r="B79" s="0">
-        <v>232.96</v>
+        <v>232.58</v>
       </c>
     </row>
     <row r="80">
@@ -1080,7 +1224,7 @@
         <v>80</v>
       </c>
       <c r="B80" s="0">
-        <v>231.05</v>
+        <v>230.68</v>
       </c>
     </row>
     <row r="81">
@@ -1088,7 +1232,7 @@
         <v>81</v>
       </c>
       <c r="B81" s="0">
-        <v>243.93</v>
+        <v>243.53</v>
       </c>
     </row>
     <row r="82">
@@ -1096,7 +1240,7 @@
         <v>82</v>
       </c>
       <c r="B82" s="0">
-        <v>278.37</v>
+        <v>277.92</v>
       </c>
     </row>
     <row r="83">
@@ -1104,7 +1248,7 @@
         <v>83</v>
       </c>
       <c r="B83" s="0">
-        <v>307.37</v>
+        <v>306.87</v>
       </c>
     </row>
     <row r="84">
@@ -1112,7 +1256,7 @@
         <v>84</v>
       </c>
       <c r="B84" s="0">
-        <v>320.05</v>
+        <v>319.53</v>
       </c>
     </row>
     <row r="85">
@@ -1120,7 +1264,7 @@
         <v>85</v>
       </c>
       <c r="B85" s="0">
-        <v>326.25</v>
+        <v>325.72</v>
       </c>
     </row>
     <row r="86">
@@ -1128,7 +1272,7 @@
         <v>86</v>
       </c>
       <c r="B86" s="0">
-        <v>324.42</v>
+        <v>323.89</v>
       </c>
     </row>
     <row r="87">
@@ -1136,7 +1280,7 @@
         <v>87</v>
       </c>
       <c r="B87" s="0">
-        <v>320.89</v>
+        <v>320.36</v>
       </c>
     </row>
     <row r="88">
@@ -1144,7 +1288,7 @@
         <v>88</v>
       </c>
       <c r="B88" s="0">
-        <v>323.38</v>
+        <v>322.86</v>
       </c>
     </row>
     <row r="89">
@@ -1152,7 +1296,7 @@
         <v>89</v>
       </c>
       <c r="B89" s="0">
-        <v>325.35</v>
+        <v>324.82</v>
       </c>
     </row>
     <row r="90">
@@ -1160,7 +1304,7 @@
         <v>90</v>
       </c>
       <c r="B90" s="0">
-        <v>343.28</v>
+        <v>342.72</v>
       </c>
     </row>
     <row r="91">
@@ -1168,7 +1312,7 @@
         <v>91</v>
       </c>
       <c r="B91" s="0">
-        <v>367.08</v>
+        <v>366.48</v>
       </c>
     </row>
     <row r="92">
@@ -1176,7 +1320,7 @@
         <v>92</v>
       </c>
       <c r="B92" s="0">
-        <v>322.11</v>
+        <v>321.58</v>
       </c>
     </row>
     <row r="93">
@@ -1184,7 +1328,7 @@
         <v>93</v>
       </c>
       <c r="B93" s="0">
-        <v>319.09</v>
+        <v>318.57</v>
       </c>
     </row>
     <row r="94">
@@ -1192,7 +1336,7 @@
         <v>94</v>
       </c>
       <c r="B94" s="0">
-        <v>284.67</v>
+        <v>284.2</v>
       </c>
     </row>
     <row r="95">
@@ -1200,7 +1344,7 @@
         <v>95</v>
       </c>
       <c r="B95" s="0">
-        <v>294.36</v>
+        <v>293.88</v>
       </c>
     </row>
     <row r="96">
@@ -1208,7 +1352,7 @@
         <v>96</v>
       </c>
       <c r="B96" s="0">
-        <v>280.94</v>
+        <v>280.48</v>
       </c>
     </row>
     <row r="97">
@@ -1216,7 +1360,7 @@
         <v>97</v>
       </c>
       <c r="B97" s="0">
-        <v>261.86</v>
+        <v>261.43</v>
       </c>
     </row>
     <row r="98">
@@ -1224,7 +1368,7 @@
         <v>98</v>
       </c>
       <c r="B98" s="0">
-        <v>223.7</v>
+        <v>223.34</v>
       </c>
     </row>
     <row r="99">
@@ -1232,7 +1376,7 @@
         <v>99</v>
       </c>
       <c r="B99" s="0">
-        <v>208.47</v>
+        <v>208.13</v>
       </c>
     </row>
     <row r="100">
@@ -1240,7 +1384,7 @@
         <v>100</v>
       </c>
       <c r="B100" s="0">
-        <v>196.26</v>
+        <v>195.94</v>
       </c>
     </row>
     <row r="101">
@@ -1248,7 +1392,7 @@
         <v>101</v>
       </c>
       <c r="B101" s="0">
-        <v>193.35</v>
+        <v>193.03</v>
       </c>
     </row>
     <row r="102">
@@ -1256,7 +1400,7 @@
         <v>102</v>
       </c>
       <c r="B102" s="0">
-        <v>178.45</v>
+        <v>178.16</v>
       </c>
     </row>
     <row r="103">
@@ -1264,7 +1408,7 @@
         <v>103</v>
       </c>
       <c r="B103" s="0">
-        <v>266.47</v>
+        <v>266.03</v>
       </c>
     </row>
     <row r="104">
@@ -1272,7 +1416,7 @@
         <v>104</v>
       </c>
       <c r="B104" s="0">
-        <v>287.51</v>
+        <v>287.04</v>
       </c>
     </row>
     <row r="105">
@@ -1280,7 +1424,7 @@
         <v>105</v>
       </c>
       <c r="B105" s="0">
-        <v>323.92</v>
+        <v>323.39</v>
       </c>
     </row>
     <row r="106">
@@ -1288,7 +1432,7 @@
         <v>106</v>
       </c>
       <c r="B106" s="0">
-        <v>314.7</v>
+        <v>314.19</v>
       </c>
     </row>
     <row r="107">
@@ -1296,7 +1440,7 @@
         <v>107</v>
       </c>
       <c r="B107" s="0">
-        <v>327.12</v>
+        <v>326.59</v>
       </c>
     </row>
     <row r="108">
@@ -1304,7 +1448,7 @@
         <v>108</v>
       </c>
       <c r="B108" s="0">
-        <v>341.32</v>
+        <v>340.76</v>
       </c>
     </row>
     <row r="109">
@@ -1312,7 +1456,7 @@
         <v>109</v>
       </c>
       <c r="B109" s="0">
-        <v>358.63</v>
+        <v>358.04</v>
       </c>
     </row>
     <row r="110">
@@ -1320,7 +1464,7 @@
         <v>110</v>
       </c>
       <c r="B110" s="0">
-        <v>352.96</v>
+        <v>352.38</v>
       </c>
     </row>
     <row r="111">
@@ -1328,7 +1472,7 @@
         <v>111</v>
       </c>
       <c r="B111" s="0">
-        <v>348.92</v>
+        <v>348.35</v>
       </c>
     </row>
     <row r="112">
@@ -1336,7 +1480,7 @@
         <v>112</v>
       </c>
       <c r="B112" s="0">
-        <v>366.29</v>
+        <v>365.69</v>
       </c>
     </row>
     <row r="113">
@@ -1344,7 +1488,7 @@
         <v>113</v>
       </c>
       <c r="B113" s="0">
-        <v>447.15</v>
+        <v>446.42</v>
       </c>
     </row>
     <row r="114">
@@ -1352,7 +1496,7 @@
         <v>114</v>
       </c>
       <c r="B114" s="0">
-        <v>458.4</v>
+        <v>457.65</v>
       </c>
     </row>
     <row r="115">
@@ -1360,7 +1504,7 @@
         <v>115</v>
       </c>
       <c r="B115" s="0">
-        <v>485.2</v>
+        <v>484.41</v>
       </c>
     </row>
     <row r="116">
@@ -1368,7 +1512,7 @@
         <v>116</v>
       </c>
       <c r="B116" s="0">
-        <v>460.97</v>
+        <v>460.22</v>
       </c>
     </row>
     <row r="117">
@@ -1376,7 +1520,7 @@
         <v>117</v>
       </c>
       <c r="B117" s="0">
-        <v>455.4</v>
+        <v>454.66</v>
       </c>
     </row>
     <row r="118">
@@ -1384,7 +1528,7 @@
         <v>118</v>
       </c>
       <c r="B118" s="0">
-        <v>417.5</v>
+        <v>416.82</v>
       </c>
     </row>
     <row r="119">
@@ -1392,7 +1536,7 @@
         <v>119</v>
       </c>
       <c r="B119" s="0">
-        <v>330.32</v>
+        <v>329.78</v>
       </c>
     </row>
     <row r="120">
@@ -1400,7 +1544,7 @@
         <v>120</v>
       </c>
       <c r="B120" s="0">
-        <v>314.4</v>
+        <v>313.89</v>
       </c>
     </row>
     <row r="121">
@@ -1408,7 +1552,391 @@
         <v>121</v>
       </c>
       <c r="B121" s="0">
-        <v>299.79</v>
+        <v>299.3</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B122" s="0">
+        <v>208.46</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B123" s="0">
+        <v>152.32</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B124" s="0">
+        <v>96.87</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B125" s="0">
+        <v>98.98</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B126" s="0">
+        <v>152.48</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B127" s="0">
+        <v>300.26</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B128" s="0">
+        <v>325.48</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B129" s="0">
+        <v>491.85</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B130" s="0">
+        <v>484.14</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B131" s="0">
+        <v>488.66</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B132" s="0">
+        <v>493.34</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B133" s="0">
+        <v>490.45</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B134" s="0">
+        <v>494.17</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B135" s="0">
+        <v>485.61</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B136" s="0">
+        <v>499.27</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B137" s="0">
+        <v>494.03</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B138" s="0">
+        <v>502.4</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B139" s="0">
+        <v>521.86</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B140" s="0">
+        <v>494.13</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B141" s="0">
+        <v>455.3</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B142" s="0">
+        <v>401.62</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B143" s="0">
+        <v>347.25</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B144" s="0">
+        <v>326.56</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B145" s="0">
+        <v>290.8</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B146" s="0">
+        <v>288.2</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B147" s="0">
+        <v>256.76</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B148" s="0">
+        <v>222.11</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B149" s="0">
+        <v>217.81</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B150" s="0">
+        <v>250.72</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B151" s="0">
+        <v>282.55</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B152" s="0">
+        <v>307.08</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B153" s="0">
+        <v>413.82</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B154" s="0">
+        <v>441.29</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B155" s="0">
+        <v>429.48</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B156" s="0">
+        <v>412.26</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B157" s="0">
+        <v>387.29</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B158" s="0">
+        <v>413.89</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B159" s="0">
+        <v>374.49</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B160" s="0">
+        <v>444.48</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B161" s="0">
+        <v>475.72</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B162" s="0">
+        <v>494.59</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B163" s="0">
+        <v>456.68</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B164" s="0">
+        <v>435.7</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B165" s="0">
+        <v>423.04</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B166" s="0">
+        <v>445.31</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B167" s="0">
+        <v>356.35</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B168" s="0">
+        <v>319.7</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B169" s="0">
+        <v>296.73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>